<commit_message>
added new features in New leagues
</commit_message>
<xml_diff>
--- a/Divisions/Roundmatrix.xlsx
+++ b/Divisions/Roundmatrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="b1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <sheet name="sc3" sheetId="20" r:id="rId20"/>
     <sheet name="t1" sheetId="21" r:id="rId21"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -4022,7 +4022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
@@ -9402,9 +9402,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="23" width="4.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -20031,7 +20039,7 @@
   <dimension ref="A1:W21"/>
   <sheetViews>
     <sheetView zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated new league divs
</commit_message>
<xml_diff>
--- a/Divisions/Roundmatrix.xlsx
+++ b/Divisions/Roundmatrix.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1667" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1668" uniqueCount="495">
   <si>
     <t>b1_teams</t>
   </si>
@@ -19997,6 +19997,9 @@
       <c r="AQ1" t="s">
         <v>139</v>
       </c>
+      <c r="AR1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -20128,6 +20131,9 @@
       <c r="AQ2" t="n">
         <v>22.0</v>
       </c>
+      <c r="AR2" t="n">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -20259,6 +20265,9 @@
       <c r="AQ3" t="n">
         <v>1.0</v>
       </c>
+      <c r="AR3" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -20390,6 +20399,9 @@
       <c r="AQ4" t="n">
         <v>19.0</v>
       </c>
+      <c r="AR4" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -20521,6 +20533,9 @@
       <c r="AQ5" t="n">
         <v>10.0</v>
       </c>
+      <c r="AR5" t="n">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -20652,6 +20667,9 @@
       <c r="AQ6" t="n">
         <v>9.0</v>
       </c>
+      <c r="AR6" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -20783,6 +20801,9 @@
       <c r="AQ7" t="n">
         <v>2.0</v>
       </c>
+      <c r="AR7" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -20914,6 +20935,9 @@
       <c r="AQ8" t="n">
         <v>21.0</v>
       </c>
+      <c r="AR8" t="n">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -21045,6 +21069,9 @@
       <c r="AQ9" t="n">
         <v>5.0</v>
       </c>
+      <c r="AR9" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -21176,6 +21203,9 @@
       <c r="AQ10" t="n">
         <v>11.0</v>
       </c>
+      <c r="AR10" t="n">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -21307,6 +21337,9 @@
       <c r="AQ11" t="n">
         <v>14.0</v>
       </c>
+      <c r="AR11" t="n">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -21438,6 +21471,9 @@
       <c r="AQ12" t="n">
         <v>6.0</v>
       </c>
+      <c r="AR12" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -21569,6 +21605,9 @@
       <c r="AQ13" t="n">
         <v>12.0</v>
       </c>
+      <c r="AR13" t="n">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -21700,6 +21739,9 @@
       <c r="AQ14" t="n">
         <v>16.0</v>
       </c>
+      <c r="AR14" t="n">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -21831,6 +21873,9 @@
       <c r="AQ15" t="n">
         <v>18.0</v>
       </c>
+      <c r="AR15" t="n">
+        <v>18.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -21962,6 +22007,9 @@
       <c r="AQ16" t="n">
         <v>15.0</v>
       </c>
+      <c r="AR16" t="n">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -22093,6 +22141,9 @@
       <c r="AQ17" t="n">
         <v>7.0</v>
       </c>
+      <c r="AR17" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -22224,6 +22275,9 @@
       <c r="AQ18" t="n">
         <v>8.0</v>
       </c>
+      <c r="AR18" t="n">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -22355,6 +22409,9 @@
       <c r="AQ19" t="n">
         <v>20.0</v>
       </c>
+      <c r="AR19" t="n">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -22486,6 +22543,9 @@
       <c r="AQ20" t="n">
         <v>17.0</v>
       </c>
+      <c r="AR20" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -22617,6 +22677,9 @@
       <c r="AQ21" t="n">
         <v>4.0</v>
       </c>
+      <c r="AR21" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -22748,6 +22811,9 @@
       <c r="AQ22" t="n">
         <v>3.0</v>
       </c>
+      <c r="AR22" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -22878,6 +22944,9 @@
       </c>
       <c r="AQ23" t="n">
         <v>13.0</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added goalscorers and results test data
</commit_message>
<xml_diff>
--- a/Divisions/Roundmatrix.xlsx
+++ b/Divisions/Roundmatrix.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="470">
   <si>
     <t>b1_teams</t>
   </si>
@@ -9563,6 +9563,9 @@
       <c r="Q1" t="s">
         <v>15</v>
       </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -9616,6 +9619,9 @@
       <c r="Q2" t="n">
         <v>1.0</v>
       </c>
+      <c r="R2" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -9669,6 +9675,9 @@
       <c r="Q3" t="n">
         <v>8.0</v>
       </c>
+      <c r="R3" t="n">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -9722,6 +9731,9 @@
       <c r="Q4" t="n">
         <v>10.0</v>
       </c>
+      <c r="R4" t="n">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -9775,6 +9787,9 @@
       <c r="Q5" t="n">
         <v>2.0</v>
       </c>
+      <c r="R5" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -9828,6 +9843,9 @@
       <c r="Q6" t="n">
         <v>6.0</v>
       </c>
+      <c r="R6" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -9881,6 +9899,9 @@
       <c r="Q7" t="n">
         <v>4.0</v>
       </c>
+      <c r="R7" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -9934,6 +9955,9 @@
       <c r="Q8" t="n">
         <v>9.0</v>
       </c>
+      <c r="R8" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -9987,6 +10011,9 @@
       <c r="Q9" t="n">
         <v>7.0</v>
       </c>
+      <c r="R9" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -10040,6 +10067,9 @@
       <c r="Q10" t="n">
         <v>21.0</v>
       </c>
+      <c r="R10" t="n">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -10093,6 +10123,9 @@
       <c r="Q11" t="n">
         <v>3.0</v>
       </c>
+      <c r="R11" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -10146,6 +10179,9 @@
       <c r="Q12" t="n">
         <v>12.0</v>
       </c>
+      <c r="R12" t="n">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -10199,6 +10235,9 @@
       <c r="Q13" t="n">
         <v>5.0</v>
       </c>
+      <c r="R13" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -10252,6 +10291,9 @@
       <c r="Q14" t="n">
         <v>19.0</v>
       </c>
+      <c r="R14" t="n">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -10305,6 +10347,9 @@
       <c r="Q15" t="n">
         <v>22.0</v>
       </c>
+      <c r="R15" t="n">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -10358,6 +10403,9 @@
       <c r="Q16" t="n">
         <v>20.0</v>
       </c>
+      <c r="R16" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
@@ -10411,6 +10459,9 @@
       <c r="Q17" t="n">
         <v>16.0</v>
       </c>
+      <c r="R17" t="n">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -10464,6 +10515,9 @@
       <c r="Q18" t="n">
         <v>17.0</v>
       </c>
+      <c r="R18" t="n">
+        <v>17.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -10517,6 +10571,9 @@
       <c r="Q19" t="n">
         <v>14.0</v>
       </c>
+      <c r="R19" t="n">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -10570,6 +10627,9 @@
       <c r="Q20" t="n">
         <v>11.0</v>
       </c>
+      <c r="R20" t="n">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -10623,6 +10683,9 @@
       <c r="Q21" t="n">
         <v>15.0</v>
       </c>
+      <c r="R21" t="n">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -10676,6 +10739,9 @@
       <c r="Q22" t="n">
         <v>13.0</v>
       </c>
+      <c r="R22" t="n">
+        <v>10.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -10727,6 +10793,9 @@
         <v>15.0</v>
       </c>
       <c r="Q23" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="R23" t="n">
         <v>18.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added cloned prediction market calculator
</commit_message>
<xml_diff>
--- a/Divisions/Roundmatrix.xlsx
+++ b/Divisions/Roundmatrix.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1187" uniqueCount="471">
   <si>
     <t>b1_teams</t>
   </si>
@@ -630,6 +630,9 @@
   </si>
   <si>
     <t>ec_teams</t>
+  </si>
+  <si>
+    <t>X22</t>
   </si>
   <si>
     <t>Aldershot</t>
@@ -2628,7 +2631,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2681,7 +2684,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C2" t="n">
         <v>15.0</v>
@@ -2734,7 +2737,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C3" t="n">
         <v>16.0</v>
@@ -2787,7 +2790,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C4" t="n">
         <v>17.0</v>
@@ -2840,7 +2843,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C5" t="n">
         <v>7.0</v>
@@ -2893,7 +2896,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C6" t="n">
         <v>1.0</v>
@@ -2946,7 +2949,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
         <v>2.0</v>
@@ -2999,7 +3002,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C8" t="n">
         <v>8.0</v>
@@ -3052,7 +3055,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C9" t="n">
         <v>3.0</v>
@@ -3105,7 +3108,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C10" t="n">
         <v>4.0</v>
@@ -3158,7 +3161,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C11" t="n">
         <v>9.0</v>
@@ -3211,7 +3214,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C12" t="n">
         <v>5.0</v>
@@ -3264,7 +3267,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C13" t="n">
         <v>18.0</v>
@@ -3317,7 +3320,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C14" t="n">
         <v>6.0</v>
@@ -3370,7 +3373,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C15" t="n">
         <v>10.0</v>
@@ -3423,7 +3426,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C16" t="n">
         <v>19.0</v>
@@ -3476,7 +3479,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C17" t="n">
         <v>11.0</v>
@@ -3529,7 +3532,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C18" t="n">
         <v>12.0</v>
@@ -3582,7 +3585,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C19" t="n">
         <v>13.0</v>
@@ -3635,7 +3638,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="C20" t="n">
         <v>20.0</v>
@@ -3688,7 +3691,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C21" t="n">
         <v>14.0</v>
@@ -3752,7 +3755,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -3799,7 +3802,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -3846,7 +3849,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C3" t="n">
         <v>2.0</v>
@@ -3893,7 +3896,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C4" t="n">
         <v>7.0</v>
@@ -3940,7 +3943,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -3987,7 +3990,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C6" t="n">
         <v>9.0</v>
@@ -4034,7 +4037,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C7" t="n">
         <v>10.0</v>
@@ -4081,7 +4084,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C8" t="n">
         <v>11.0</v>
@@ -4128,7 +4131,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C9" t="n">
         <v>12.0</v>
@@ -4175,7 +4178,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C10" t="n">
         <v>13.0</v>
@@ -4222,7 +4225,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C11" t="n">
         <v>4.0</v>
@@ -4269,7 +4272,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C12" t="n">
         <v>5.0</v>
@@ -4316,7 +4319,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C13" t="n">
         <v>14.0</v>
@@ -4363,7 +4366,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C14" t="n">
         <v>6.0</v>
@@ -4410,7 +4413,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C15" t="n">
         <v>8.0</v>
@@ -4468,7 +4471,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -4521,7 +4524,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -4574,7 +4577,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C3" t="n">
         <v>11.0</v>
@@ -4627,7 +4630,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C4" t="n">
         <v>12.0</v>
@@ -4680,7 +4683,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C5" t="n">
         <v>13.0</v>
@@ -4733,7 +4736,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -4786,7 +4789,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="C7" t="n">
         <v>3.0</v>
@@ -4839,7 +4842,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C8" t="n">
         <v>4.0</v>
@@ -4892,7 +4895,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C9" t="n">
         <v>5.0</v>
@@ -4945,7 +4948,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C10" t="n">
         <v>14.0</v>
@@ -4998,7 +5001,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C11" t="n">
         <v>6.0</v>
@@ -5051,7 +5054,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C12" t="n">
         <v>15.0</v>
@@ -5104,7 +5107,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C13" t="n">
         <v>7.0</v>
@@ -5157,7 +5160,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C14" t="n">
         <v>8.0</v>
@@ -5210,7 +5213,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C15" t="n">
         <v>16.0</v>
@@ -5263,7 +5266,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C16" t="n">
         <v>17.0</v>
@@ -5316,7 +5319,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C17" t="n">
         <v>18.0</v>
@@ -5369,7 +5372,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C18" t="n">
         <v>9.0</v>
@@ -5422,7 +5425,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C19" t="n">
         <v>10.0</v>
@@ -5475,7 +5478,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C20" t="n">
         <v>19.0</v>
@@ -5528,7 +5531,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C21" t="n">
         <v>20.0</v>
@@ -5592,7 +5595,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -5632,6 +5635,12 @@
       </c>
       <c r="O1" t="s">
         <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="2">
@@ -5639,7 +5648,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -5678,6 +5687,12 @@
         <v>6.0</v>
       </c>
       <c r="O2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="Q2" t="n">
         <v>9.0</v>
       </c>
     </row>
@@ -5686,7 +5701,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C3" t="n">
         <v>9.0</v>
@@ -5726,6 +5741,12 @@
       </c>
       <c r="O3" t="n">
         <v>6.0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="4">
@@ -5733,7 +5754,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C4" t="n">
         <v>13.0</v>
@@ -5773,6 +5794,12 @@
       </c>
       <c r="O4" t="n">
         <v>15.0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>16.0</v>
       </c>
     </row>
     <row r="5">
@@ -5780,7 +5807,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C5" t="n">
         <v>2.0</v>
@@ -5820,6 +5847,12 @@
       </c>
       <c r="O5" t="n">
         <v>7.0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="6">
@@ -5827,7 +5860,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C6" t="n">
         <v>10.0</v>
@@ -5867,6 +5900,12 @@
       </c>
       <c r="O6" t="n">
         <v>10.0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>11.0</v>
       </c>
     </row>
     <row r="7">
@@ -5874,7 +5913,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C7" t="n">
         <v>3.0</v>
@@ -5914,6 +5953,12 @@
       </c>
       <c r="O7" t="n">
         <v>11.0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="8">
@@ -5921,7 +5966,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C8" t="n">
         <v>11.0</v>
@@ -5961,6 +6006,12 @@
       </c>
       <c r="O8" t="n">
         <v>18.0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="9">
@@ -5968,7 +6019,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C9" t="n">
         <v>4.0</v>
@@ -6008,6 +6059,12 @@
       </c>
       <c r="O9" t="n">
         <v>16.0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>15.0</v>
       </c>
     </row>
     <row r="10">
@@ -6015,7 +6072,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C10" t="n">
         <v>5.0</v>
@@ -6054,6 +6111,12 @@
         <v>1.0</v>
       </c>
       <c r="O10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="Q10" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -6062,7 +6125,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C11" t="n">
         <v>6.0</v>
@@ -6102,6 +6165,12 @@
       </c>
       <c r="O11" t="n">
         <v>3.0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="12">
@@ -6109,7 +6178,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C12" t="n">
         <v>14.0</v>
@@ -6149,6 +6218,12 @@
       </c>
       <c r="O12" t="n">
         <v>17.0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="13">
@@ -6156,7 +6231,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C13" t="n">
         <v>7.0</v>
@@ -6196,6 +6271,12 @@
       </c>
       <c r="O13" t="n">
         <v>12.0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="14">
@@ -6203,7 +6284,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C14" t="n">
         <v>12.0</v>
@@ -6243,6 +6324,12 @@
       </c>
       <c r="O14" t="n">
         <v>4.0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="15">
@@ -6250,7 +6337,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="C15" t="n">
         <v>15.0</v>
@@ -6289,6 +6376,12 @@
         <v>20.0</v>
       </c>
       <c r="O15" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="Q15" t="n">
         <v>20.0</v>
       </c>
     </row>
@@ -6297,7 +6390,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C16" t="n">
         <v>16.0</v>
@@ -6336,6 +6429,12 @@
         <v>14.0</v>
       </c>
       <c r="O16" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="P16" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="Q16" t="n">
         <v>13.0</v>
       </c>
     </row>
@@ -6344,7 +6443,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C17" t="n">
         <v>8.0</v>
@@ -6383,6 +6482,12 @@
         <v>3.0</v>
       </c>
       <c r="O17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="P17" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="Q17" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -6391,7 +6496,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C18" t="n">
         <v>17.0</v>
@@ -6431,6 +6536,12 @@
       </c>
       <c r="O18" t="n">
         <v>14.0</v>
+      </c>
+      <c r="P18" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>18.0</v>
       </c>
     </row>
     <row r="19">
@@ -6438,7 +6549,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C19" t="n">
         <v>18.0</v>
@@ -6478,6 +6589,12 @@
       </c>
       <c r="O19" t="n">
         <v>8.0</v>
+      </c>
+      <c r="P19" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="20">
@@ -6485,7 +6602,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="C20" t="n">
         <v>19.0</v>
@@ -6525,6 +6642,12 @@
       </c>
       <c r="O20" t="n">
         <v>5.0</v>
+      </c>
+      <c r="P20" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="21">
@@ -6532,7 +6655,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C21" t="n">
         <v>20.0</v>
@@ -6571,6 +6694,12 @@
         <v>19.0</v>
       </c>
       <c r="O21" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="P21" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="Q21" t="n">
         <v>19.0</v>
       </c>
     </row>
@@ -6590,7 +6719,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -6640,7 +6769,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -6690,7 +6819,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="C3" t="n">
         <v>2.0</v>
@@ -6740,7 +6869,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C4" t="n">
         <v>13.0</v>
@@ -6790,7 +6919,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -6840,7 +6969,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C6" t="n">
         <v>14.0</v>
@@ -6890,7 +7019,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="C7" t="n">
         <v>4.0</v>
@@ -6940,7 +7069,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C8" t="n">
         <v>15.0</v>
@@ -6990,7 +7119,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="C9" t="n">
         <v>16.0</v>
@@ -7040,7 +7169,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C10" t="n">
         <v>7.0</v>
@@ -7090,7 +7219,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C11" t="n">
         <v>8.0</v>
@@ -7140,7 +7269,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C12" t="n">
         <v>17.0</v>
@@ -7190,7 +7319,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C13" t="n">
         <v>5.0</v>
@@ -7240,7 +7369,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C14" t="n">
         <v>9.0</v>
@@ -7290,7 +7419,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C15" t="n">
         <v>6.0</v>
@@ -7340,7 +7469,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C16" t="n">
         <v>10.0</v>
@@ -7390,7 +7519,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C17" t="n">
         <v>18.0</v>
@@ -7440,7 +7569,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C18" t="n">
         <v>11.0</v>
@@ -7490,7 +7619,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C19" t="n">
         <v>12.0</v>
@@ -7551,7 +7680,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -7598,7 +7727,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C2" t="n">
         <v>12.0</v>
@@ -7645,7 +7774,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -7692,7 +7821,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -7739,7 +7868,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C5" t="n">
         <v>8.0</v>
@@ -7786,7 +7915,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C6" t="n">
         <v>13.0</v>
@@ -7833,7 +7962,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C7" t="n">
         <v>3.0</v>
@@ -7880,7 +8009,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C8" t="n">
         <v>14.0</v>
@@ -7927,7 +8056,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C9" t="n">
         <v>4.0</v>
@@ -7974,7 +8103,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C10" t="n">
         <v>5.0</v>
@@ -8021,7 +8150,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C11" t="n">
         <v>15.0</v>
@@ -8068,7 +8197,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C12" t="n">
         <v>16.0</v>
@@ -8115,7 +8244,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C13" t="n">
         <v>17.0</v>
@@ -8162,7 +8291,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C14" t="n">
         <v>6.0</v>
@@ -8209,7 +8338,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C15" t="n">
         <v>18.0</v>
@@ -8256,7 +8385,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C16" t="n">
         <v>9.0</v>
@@ -8303,7 +8432,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C17" t="n">
         <v>10.0</v>
@@ -8350,7 +8479,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="C18" t="n">
         <v>11.0</v>
@@ -8397,7 +8526,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C19" t="n">
         <v>7.0</v>
@@ -8455,7 +8584,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -8505,7 +8634,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C2" t="n">
         <v>14.0</v>
@@ -8555,7 +8684,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C3" t="n">
         <v>8.0</v>
@@ -8605,7 +8734,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -8655,7 +8784,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="C5" t="n">
         <v>9.0</v>
@@ -8705,7 +8834,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C6" t="n">
         <v>2.0</v>
@@ -8755,7 +8884,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C7" t="n">
         <v>15.0</v>
@@ -8805,7 +8934,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C8" t="n">
         <v>10.0</v>
@@ -8855,7 +8984,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C9" t="n">
         <v>16.0</v>
@@ -8905,7 +9034,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C10" t="n">
         <v>11.0</v>
@@ -8955,7 +9084,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C11" t="n">
         <v>17.0</v>
@@ -9005,7 +9134,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="C12" t="n">
         <v>18.0</v>
@@ -9055,7 +9184,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C13" t="n">
         <v>12.0</v>
@@ -9105,7 +9234,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C14" t="n">
         <v>3.0</v>
@@ -9155,7 +9284,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C15" t="n">
         <v>4.0</v>
@@ -9205,7 +9334,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C16" t="n">
         <v>19.0</v>
@@ -9255,7 +9384,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C17" t="n">
         <v>5.0</v>
@@ -9305,7 +9434,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C18" t="n">
         <v>6.0</v>
@@ -9355,7 +9484,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C19" t="n">
         <v>20.0</v>
@@ -9405,7 +9534,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C20" t="n">
         <v>13.0</v>
@@ -9455,7 +9584,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C21" t="n">
         <v>7.0</v>
@@ -9516,7 +9645,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -9565,6 +9694,12 @@
       </c>
       <c r="R1" t="s">
         <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2">
@@ -9572,7 +9707,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -9620,6 +9755,12 @@
         <v>1.0</v>
       </c>
       <c r="R2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="T2" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -9628,7 +9769,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C3" t="n">
         <v>2.0</v>
@@ -9677,6 +9818,12 @@
       </c>
       <c r="R3" t="n">
         <v>11.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="4">
@@ -9684,7 +9831,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C4" t="n">
         <v>3.0</v>
@@ -9732,6 +9879,12 @@
         <v>10.0</v>
       </c>
       <c r="R4" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="T4" t="n">
         <v>8.0</v>
       </c>
     </row>
@@ -9740,7 +9893,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C5" t="n">
         <v>4.0</v>
@@ -9788,6 +9941,12 @@
         <v>2.0</v>
       </c>
       <c r="R5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="T5" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -9796,7 +9955,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C6" t="n">
         <v>15.0</v>
@@ -9845,6 +10004,12 @@
       </c>
       <c r="R6" t="n">
         <v>6.0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="7">
@@ -9852,7 +10017,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C7" t="n">
         <v>5.0</v>
@@ -9901,6 +10066,12 @@
       </c>
       <c r="R7" t="n">
         <v>4.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="8">
@@ -9908,7 +10079,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C8" t="n">
         <v>6.0</v>
@@ -9956,6 +10127,12 @@
         <v>9.0</v>
       </c>
       <c r="R8" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="T8" t="n">
         <v>7.0</v>
       </c>
     </row>
@@ -9964,7 +10141,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C9" t="n">
         <v>9.0</v>
@@ -10013,6 +10190,12 @@
       </c>
       <c r="R9" t="n">
         <v>9.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>11.0</v>
       </c>
     </row>
     <row r="10">
@@ -10020,7 +10203,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="C10" t="n">
         <v>16.0</v>
@@ -10069,6 +10252,12 @@
       </c>
       <c r="R10" t="n">
         <v>21.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>22.0</v>
       </c>
     </row>
     <row r="11">
@@ -10076,7 +10265,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C11" t="n">
         <v>10.0</v>
@@ -10124,6 +10313,12 @@
         <v>3.0</v>
       </c>
       <c r="R11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="T11" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -10132,7 +10327,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C12" t="n">
         <v>17.0</v>
@@ -10181,6 +10376,12 @@
       </c>
       <c r="R12" t="n">
         <v>13.0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="T12" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="13">
@@ -10188,7 +10389,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C13" t="n">
         <v>11.0</v>
@@ -10236,6 +10437,12 @@
         <v>5.0</v>
       </c>
       <c r="R13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="T13" t="n">
         <v>5.0</v>
       </c>
     </row>
@@ -10244,7 +10451,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C14" t="n">
         <v>18.0</v>
@@ -10293,6 +10500,12 @@
       </c>
       <c r="R14" t="n">
         <v>20.0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="T14" t="n">
+        <v>18.0</v>
       </c>
     </row>
     <row r="15">
@@ -10300,7 +10513,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C15" t="n">
         <v>19.0</v>
@@ -10349,6 +10562,12 @@
       </c>
       <c r="R15" t="n">
         <v>22.0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="T15" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="16">
@@ -10356,7 +10575,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C16" t="n">
         <v>12.0</v>
@@ -10405,6 +10624,12 @@
       </c>
       <c r="R16" t="n">
         <v>19.0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="T16" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="17">
@@ -10412,7 +10637,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C17" t="n">
         <v>20.0</v>
@@ -10461,6 +10686,12 @@
       </c>
       <c r="R17" t="n">
         <v>16.0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="T17" t="n">
+        <v>13.0</v>
       </c>
     </row>
     <row r="18">
@@ -10468,7 +10699,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="C18" t="n">
         <v>7.0</v>
@@ -10517,6 +10748,12 @@
       </c>
       <c r="R18" t="n">
         <v>17.0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="T18" t="n">
+        <v>20.0</v>
       </c>
     </row>
     <row r="19">
@@ -10524,7 +10761,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C19" t="n">
         <v>21.0</v>
@@ -10573,6 +10810,12 @@
       </c>
       <c r="R19" t="n">
         <v>15.0</v>
+      </c>
+      <c r="S19" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="T19" t="n">
+        <v>19.0</v>
       </c>
     </row>
     <row r="20">
@@ -10580,7 +10823,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C20" t="n">
         <v>13.0</v>
@@ -10629,6 +10872,12 @@
       </c>
       <c r="R20" t="n">
         <v>12.0</v>
+      </c>
+      <c r="S20" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="T20" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="21">
@@ -10636,7 +10885,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C21" t="n">
         <v>22.0</v>
@@ -10685,6 +10934,12 @@
       </c>
       <c r="R21" t="n">
         <v>14.0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="T21" t="n">
+        <v>16.0</v>
       </c>
     </row>
     <row r="22">
@@ -10692,7 +10947,7 @@
         <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C22" t="n">
         <v>8.0</v>
@@ -10741,6 +10996,12 @@
       </c>
       <c r="R22" t="n">
         <v>10.0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="T22" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="23">
@@ -10748,7 +11009,7 @@
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C23" t="n">
         <v>14.0</v>
@@ -10797,6 +11058,12 @@
       </c>
       <c r="R23" t="n">
         <v>18.0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="T23" t="n">
+        <v>15.0</v>
       </c>
     </row>
   </sheetData>
@@ -10815,7 +11082,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -10871,7 +11138,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C2" t="n">
         <v>8.0</v>
@@ -10927,7 +11194,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="C3" t="n">
         <v>1.0</v>
@@ -10983,7 +11250,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C4" t="n">
         <v>6.0</v>
@@ -11039,7 +11306,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C5" t="n">
         <v>2.0</v>
@@ -11095,7 +11362,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C6" t="n">
         <v>3.0</v>
@@ -11151,7 +11418,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C7" t="n">
         <v>7.0</v>
@@ -11207,7 +11474,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C8" t="n">
         <v>9.0</v>
@@ -11263,7 +11530,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C9" t="n">
         <v>4.0</v>
@@ -11319,7 +11586,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C10" t="n">
         <v>5.0</v>
@@ -11375,7 +11642,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C11" t="n">
         <v>10.0</v>
@@ -11431,7 +11698,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C12" t="n">
         <v>11.0</v>
@@ -11487,7 +11754,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C13" t="n">
         <v>12.0</v>
@@ -11554,7 +11821,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -11603,6 +11870,9 @@
       </c>
       <c r="R1" t="s">
         <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -11610,7 +11880,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C2" t="n">
         <v>3.0</v>
@@ -11658,6 +11928,9 @@
         <v>9.0</v>
       </c>
       <c r="R2" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="S2" t="n">
         <v>9.0</v>
       </c>
     </row>
@@ -11666,7 +11939,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="C3" t="n">
         <v>4.0</v>
@@ -11714,6 +11987,9 @@
         <v>1.0</v>
       </c>
       <c r="R3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S3" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -11722,7 +11998,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -11770,6 +12046,9 @@
         <v>8.0</v>
       </c>
       <c r="R4" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="S4" t="n">
         <v>8.0</v>
       </c>
     </row>
@@ -11778,7 +12057,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C5" t="n">
         <v>9.0</v>
@@ -11826,6 +12105,9 @@
         <v>2.0</v>
       </c>
       <c r="R5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="S5" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -11834,7 +12116,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="C6" t="n">
         <v>5.0</v>
@@ -11882,6 +12164,9 @@
         <v>10.0</v>
       </c>
       <c r="R6" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="S6" t="n">
         <v>10.0</v>
       </c>
     </row>
@@ -11890,7 +12175,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C7" t="n">
         <v>6.0</v>
@@ -11939,6 +12224,9 @@
       </c>
       <c r="R7" t="n">
         <v>5.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="8">
@@ -11946,7 +12234,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C8" t="n">
         <v>7.0</v>
@@ -11995,6 +12283,9 @@
       </c>
       <c r="R8" t="n">
         <v>3.0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="9">
@@ -12002,7 +12293,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="C9" t="n">
         <v>2.0</v>
@@ -12051,6 +12342,9 @@
       </c>
       <c r="R9" t="n">
         <v>6.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="10">
@@ -12058,7 +12352,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C10" t="n">
         <v>8.0</v>
@@ -12107,6 +12401,9 @@
       </c>
       <c r="R10" t="n">
         <v>4.0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
@@ -12114,7 +12411,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C11" t="n">
         <v>10.0</v>
@@ -12162,6 +12459,9 @@
         <v>6.0</v>
       </c>
       <c r="R11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="S11" t="n">
         <v>7.0</v>
       </c>
     </row>
@@ -13199,7 +13499,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -13248,6 +13548,9 @@
       </c>
       <c r="R1" t="s">
         <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -13255,7 +13558,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C2" t="n">
         <v>1.0</v>
@@ -13303,6 +13606,9 @@
         <v>6.0</v>
       </c>
       <c r="R2" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="S2" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -13311,7 +13617,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C3" t="n">
         <v>7.0</v>
@@ -13359,6 +13665,9 @@
         <v>4.0</v>
       </c>
       <c r="R3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S3" t="n">
         <v>5.0</v>
       </c>
     </row>
@@ -13367,7 +13676,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C4" t="n">
         <v>2.0</v>
@@ -13415,6 +13724,9 @@
         <v>9.0</v>
       </c>
       <c r="R4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="S4" t="n">
         <v>9.0</v>
       </c>
     </row>
@@ -13423,7 +13735,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C5" t="n">
         <v>3.0</v>
@@ -13471,6 +13783,9 @@
         <v>1.0</v>
       </c>
       <c r="R5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S5" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -13479,7 +13794,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C6" t="n">
         <v>5.0</v>
@@ -13528,6 +13843,9 @@
       </c>
       <c r="R6" t="n">
         <v>2.0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
@@ -13535,7 +13853,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="C7" t="n">
         <v>4.0</v>
@@ -13584,6 +13902,9 @@
       </c>
       <c r="R7" t="n">
         <v>3.0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="8">
@@ -13591,7 +13912,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="C8" t="n">
         <v>8.0</v>
@@ -13639,6 +13960,9 @@
         <v>8.0</v>
       </c>
       <c r="R8" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="S8" t="n">
         <v>8.0</v>
       </c>
     </row>
@@ -13647,7 +13971,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C9" t="n">
         <v>6.0</v>
@@ -13695,6 +14019,9 @@
         <v>3.0</v>
       </c>
       <c r="R9" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="S9" t="n">
         <v>4.0</v>
       </c>
     </row>
@@ -13703,7 +14030,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C10" t="n">
         <v>9.0</v>
@@ -13751,6 +14078,9 @@
         <v>10.0</v>
       </c>
       <c r="R10" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="S10" t="n">
         <v>10.0</v>
       </c>
     </row>
@@ -13759,7 +14089,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C11" t="n">
         <v>10.0</v>
@@ -13807,6 +14137,9 @@
         <v>7.0</v>
       </c>
       <c r="R11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="S11" t="n">
         <v>7.0</v>
       </c>
     </row>
@@ -13826,7 +14159,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -13872,6 +14205,12 @@
       </c>
       <c r="Q1" t="s">
         <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2">
@@ -13879,7 +14218,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="C2" t="n">
         <v>6.0</v>
@@ -13925,6 +14264,12 @@
       </c>
       <c r="Q2" t="n">
         <v>7.0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
@@ -13932,7 +14277,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C3" t="n">
         <v>7.0</v>
@@ -13978,6 +14323,12 @@
       </c>
       <c r="Q3" t="n">
         <v>8.0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="4">
@@ -13985,7 +14336,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -14030,6 +14381,12 @@
         <v>9.0</v>
       </c>
       <c r="Q4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="S4" t="n">
         <v>9.0</v>
       </c>
     </row>
@@ -14038,7 +14395,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C5" t="n">
         <v>2.0</v>
@@ -14083,6 +14440,12 @@
         <v>1.0</v>
       </c>
       <c r="Q5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="S5" t="n">
         <v>1.0</v>
       </c>
     </row>
@@ -14091,7 +14454,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C6" t="n">
         <v>3.0</v>
@@ -14137,6 +14500,12 @@
       </c>
       <c r="Q6" t="n">
         <v>4.0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="7">
@@ -14144,7 +14513,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="C7" t="n">
         <v>8.0</v>
@@ -14189,6 +14558,12 @@
         <v>4.0</v>
       </c>
       <c r="Q7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="S7" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -14197,7 +14572,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C8" t="n">
         <v>9.0</v>
@@ -14242,6 +14617,12 @@
         <v>10.0</v>
       </c>
       <c r="Q8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="S8" t="n">
         <v>10.0</v>
       </c>
     </row>
@@ -14250,7 +14631,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C9" t="n">
         <v>4.0</v>
@@ -14296,6 +14677,12 @@
       </c>
       <c r="Q9" t="n">
         <v>5.0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="10">
@@ -14303,7 +14690,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C10" t="n">
         <v>10.0</v>
@@ -14348,6 +14735,12 @@
         <v>2.0</v>
       </c>
       <c r="Q10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="S10" t="n">
         <v>2.0</v>
       </c>
     </row>
@@ -14356,7 +14749,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C11" t="n">
         <v>5.0</v>
@@ -14402,6 +14795,12 @@
       </c>
       <c r="Q11" t="n">
         <v>6.0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>
@@ -14420,7 +14819,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -14467,7 +14866,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C2" t="n">
         <v>2.0</v>
@@ -14514,7 +14913,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C3" t="n">
         <v>3.0</v>
@@ -14561,7 +14960,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C4" t="n">
         <v>7.0</v>
@@ -14608,7 +15007,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="C5" t="n">
         <v>13.0</v>
@@ -14655,7 +15054,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C6" t="n">
         <v>4.0</v>
@@ -14702,7 +15101,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C7" t="n">
         <v>5.0</v>
@@ -14749,7 +15148,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C8" t="n">
         <v>8.0</v>
@@ -14796,7 +15195,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C9" t="n">
         <v>6.0</v>
@@ -14843,7 +15242,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C10" t="n">
         <v>9.0</v>
@@ -14890,7 +15289,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C11" t="n">
         <v>14.0</v>
@@ -14937,7 +15336,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C12" t="n">
         <v>15.0</v>
@@ -14984,7 +15383,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C13" t="n">
         <v>16.0</v>
@@ -15031,7 +15430,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C14" t="n">
         <v>17.0</v>
@@ -15078,7 +15477,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C15" t="n">
         <v>18.0</v>
@@ -15125,7 +15524,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="C16" t="n">
         <v>19.0</v>
@@ -15172,7 +15571,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C17" t="n">
         <v>10.0</v>
@@ -15219,7 +15618,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C18" t="n">
         <v>11.0</v>
@@ -15266,7 +15665,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C19" t="n">
         <v>1.0</v>
@@ -15313,7 +15712,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="C20" t="n">
         <v>12.0</v>
@@ -17761,7 +18160,7 @@
         <v>10.0</v>
       </c>
       <c r="W2" t="n">
-        <v>13.0</v>
+        <v>14.0</v>
       </c>
     </row>
     <row r="3">
@@ -18187,7 +18586,7 @@
         <v>13.0</v>
       </c>
       <c r="W8" t="n">
-        <v>11.0</v>
+        <v>12.0</v>
       </c>
     </row>
     <row r="9">
@@ -18471,7 +18870,7 @@
         <v>20.0</v>
       </c>
       <c r="W12" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
       </c>
     </row>
     <row r="13">
@@ -18826,7 +19225,7 @@
         <v>14.0</v>
       </c>
       <c r="W17" t="n">
-        <v>12.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="18">
@@ -19110,7 +19509,7 @@
         <v>12.0</v>
       </c>
       <c r="W21" t="n">
-        <v>15.0</v>
+        <v>11.0</v>
       </c>
     </row>
     <row r="22">
@@ -19472,6 +19871,9 @@
       <c r="U1" t="s">
         <v>117</v>
       </c>
+      <c r="V1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -19537,6 +19939,9 @@
       <c r="U2" t="n">
         <v>19.0</v>
       </c>
+      <c r="V2" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -19602,6 +20007,9 @@
       <c r="U3" t="n">
         <v>6.0</v>
       </c>
+      <c r="V3" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -19667,6 +20075,9 @@
       <c r="U4" t="n">
         <v>4.0</v>
       </c>
+      <c r="V4" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -19730,7 +20141,10 @@
         <v>11.0</v>
       </c>
       <c r="U5" t="n">
-        <v>13.0</v>
+        <v>12.0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="6">
@@ -19795,7 +20209,10 @@
         <v>23.0</v>
       </c>
       <c r="U6" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>22.0</v>
       </c>
     </row>
     <row r="7">
@@ -19862,6 +20279,9 @@
       <c r="U7" t="n">
         <v>20.0</v>
       </c>
+      <c r="V7" t="n">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -19925,7 +20345,10 @@
         <v>12.0</v>
       </c>
       <c r="U8" t="n">
-        <v>14.0</v>
+        <v>15.0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="9">
@@ -19990,7 +20413,10 @@
         <v>19.0</v>
       </c>
       <c r="U9" t="n">
-        <v>17.0</v>
+        <v>13.0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>15.0</v>
       </c>
     </row>
     <row r="10">
@@ -20057,6 +20483,9 @@
       <c r="U10" t="n">
         <v>7.0</v>
       </c>
+      <c r="V10" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -20120,6 +20549,9 @@
         <v>9.0</v>
       </c>
       <c r="U11" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="V11" t="n">
         <v>11.0</v>
       </c>
     </row>
@@ -20185,6 +20617,9 @@
         <v>17.0</v>
       </c>
       <c r="U12" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="V12" t="n">
         <v>18.0</v>
       </c>
     </row>
@@ -20250,7 +20685,10 @@
         <v>24.0</v>
       </c>
       <c r="U13" t="n">
-        <v>22.0</v>
+        <v>23.0</v>
+      </c>
+      <c r="V13" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="14">
@@ -20317,6 +20755,9 @@
       <c r="U14" t="n">
         <v>2.0</v>
       </c>
+      <c r="V14" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -20380,7 +20821,10 @@
         <v>13.0</v>
       </c>
       <c r="U15" t="n">
-        <v>9.0</v>
+        <v>10.0</v>
+      </c>
+      <c r="V15" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="16">
@@ -20445,6 +20889,9 @@
         <v>21.0</v>
       </c>
       <c r="U16" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="V16" t="n">
         <v>23.0</v>
       </c>
     </row>
@@ -20510,6 +20957,9 @@
         <v>22.0</v>
       </c>
       <c r="U17" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="V17" t="n">
         <v>24.0</v>
       </c>
     </row>
@@ -20575,7 +21025,10 @@
         <v>14.0</v>
       </c>
       <c r="U18" t="n">
-        <v>15.0</v>
+        <v>16.0</v>
+      </c>
+      <c r="V18" t="n">
+        <v>16.0</v>
       </c>
     </row>
     <row r="19">
@@ -20642,6 +21095,9 @@
       <c r="U19" t="n">
         <v>5.0</v>
       </c>
+      <c r="V19" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -20707,6 +21163,9 @@
       <c r="U20" t="n">
         <v>1.0</v>
       </c>
+      <c r="V20" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -20770,7 +21229,10 @@
         <v>15.0</v>
       </c>
       <c r="U21" t="n">
-        <v>10.0</v>
+        <v>11.0</v>
+      </c>
+      <c r="V21" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="22">
@@ -20837,6 +21299,9 @@
       <c r="U22" t="n">
         <v>8.0</v>
       </c>
+      <c r="V22" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
@@ -20902,6 +21367,9 @@
       <c r="U23" t="n">
         <v>3.0</v>
       </c>
+      <c r="V23" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -20965,7 +21433,10 @@
         <v>16.0</v>
       </c>
       <c r="U24" t="n">
-        <v>16.0</v>
+        <v>18.0</v>
+      </c>
+      <c r="V24" t="n">
+        <v>13.0</v>
       </c>
     </row>
     <row r="25">
@@ -21030,7 +21501,10 @@
         <v>10.0</v>
       </c>
       <c r="U25" t="n">
-        <v>12.0</v>
+        <v>14.0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -21108,6 +21582,9 @@
       <c r="U1" t="s">
         <v>117</v>
       </c>
+      <c r="V1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -21173,6 +21650,9 @@
       <c r="U2" t="n">
         <v>12.0</v>
       </c>
+      <c r="V2" t="n">
+        <v>11.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -21238,6 +21718,9 @@
       <c r="U3" t="n">
         <v>4.0</v>
       </c>
+      <c r="V3" t="n">
+        <v>4.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -21303,6 +21786,9 @@
       <c r="U4" t="n">
         <v>5.0</v>
       </c>
+      <c r="V4" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -21368,6 +21854,9 @@
       <c r="U5" t="n">
         <v>6.0</v>
       </c>
+      <c r="V5" t="n">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -21433,6 +21922,9 @@
       <c r="U6" t="n">
         <v>22.0</v>
       </c>
+      <c r="V6" t="n">
+        <v>22.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -21498,6 +21990,9 @@
       <c r="U7" t="n">
         <v>19.0</v>
       </c>
+      <c r="V7" t="n">
+        <v>19.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
@@ -21563,6 +22058,9 @@
       <c r="U8" t="n">
         <v>14.0</v>
       </c>
+      <c r="V8" t="n">
+        <v>15.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
@@ -21628,6 +22126,9 @@
       <c r="U9" t="n">
         <v>9.0</v>
       </c>
+      <c r="V9" t="n">
+        <v>12.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
@@ -21693,6 +22194,9 @@
       <c r="U10" t="n">
         <v>23.0</v>
       </c>
+      <c r="V10" t="n">
+        <v>23.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
@@ -21758,6 +22262,9 @@
       <c r="U11" t="n">
         <v>16.0</v>
       </c>
+      <c r="V11" t="n">
+        <v>16.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
@@ -21823,6 +22330,9 @@
       <c r="U12" t="n">
         <v>20.0</v>
       </c>
+      <c r="V12" t="n">
+        <v>20.0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
@@ -21888,6 +22398,9 @@
       <c r="U13" t="n">
         <v>24.0</v>
       </c>
+      <c r="V13" t="n">
+        <v>24.0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
@@ -21953,6 +22466,9 @@
       <c r="U14" t="n">
         <v>1.0</v>
       </c>
+      <c r="V14" t="n">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
@@ -22018,6 +22534,9 @@
       <c r="U15" t="n">
         <v>8.0</v>
       </c>
+      <c r="V15" t="n">
+        <v>7.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
@@ -22081,6 +22600,9 @@
         <v>19.0</v>
       </c>
       <c r="U16" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="V16" t="n">
         <v>18.0</v>
       </c>
     </row>
@@ -22148,6 +22670,9 @@
       <c r="U17" t="n">
         <v>3.0</v>
       </c>
+      <c r="V17" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
@@ -22213,6 +22738,9 @@
       <c r="U18" t="n">
         <v>21.0</v>
       </c>
+      <c r="V18" t="n">
+        <v>21.0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
@@ -22278,6 +22806,9 @@
       <c r="U19" t="n">
         <v>10.0</v>
       </c>
+      <c r="V19" t="n">
+        <v>8.0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
@@ -22343,6 +22874,9 @@
       <c r="U20" t="n">
         <v>2.0</v>
       </c>
+      <c r="V20" t="n">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
@@ -22408,6 +22942,9 @@
       <c r="U21" t="n">
         <v>15.0</v>
       </c>
+      <c r="V21" t="n">
+        <v>13.0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
@@ -22471,6 +23008,9 @@
         <v>17.0</v>
       </c>
       <c r="U22" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="V22" t="n">
         <v>17.0</v>
       </c>
     </row>
@@ -22538,6 +23078,9 @@
       <c r="U23" t="n">
         <v>7.0</v>
       </c>
+      <c r="V23" t="n">
+        <v>9.0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
@@ -22603,6 +23146,9 @@
       <c r="U24" t="n">
         <v>13.0</v>
       </c>
+      <c r="V24" t="n">
+        <v>14.0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
@@ -22667,6 +23213,9 @@
       </c>
       <c r="U25" t="n">
         <v>11.0</v>
+      </c>
+      <c r="V25" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>
@@ -22747,13 +23296,19 @@
       <c r="V1" t="s">
         <v>118</v>
       </c>
+      <c r="W1" t="s">
+        <v>119</v>
+      </c>
+      <c r="X1" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C2" t="n">
         <v>17.0</v>
@@ -22814,6 +23369,12 @@
       </c>
       <c r="V2" t="n">
         <v>18.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>15.0</v>
       </c>
     </row>
     <row r="3">
@@ -22821,7 +23382,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C3" t="n">
         <v>9.0</v>
@@ -22881,6 +23442,12 @@
         <v>17.0</v>
       </c>
       <c r="V3" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="X3" t="n">
         <v>16.0</v>
       </c>
     </row>
@@ -22889,7 +23456,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C4" t="n">
         <v>1.0</v>
@@ -22949,6 +23516,12 @@
         <v>5.0</v>
       </c>
       <c r="V4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="X4" t="n">
         <v>5.0</v>
       </c>
     </row>
@@ -22957,7 +23530,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C5" t="n">
         <v>2.0</v>
@@ -23018,6 +23591,12 @@
       </c>
       <c r="V5" t="n">
         <v>10.0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="6">
@@ -23025,7 +23604,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C6" t="n">
         <v>18.0</v>
@@ -23086,6 +23665,12 @@
       </c>
       <c r="V6" t="n">
         <v>8.0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="7">
@@ -23093,7 +23678,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C7" t="n">
         <v>10.0</v>
@@ -23153,6 +23738,12 @@
         <v>3.0</v>
       </c>
       <c r="V7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="X7" t="n">
         <v>3.0</v>
       </c>
     </row>
@@ -23161,7 +23752,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C8" t="n">
         <v>11.0</v>
@@ -23222,6 +23813,12 @@
       </c>
       <c r="V8" t="n">
         <v>9.0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>10.0</v>
       </c>
     </row>
     <row r="9">
@@ -23229,7 +23826,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C9" t="n">
         <v>12.0</v>
@@ -23289,6 +23886,12 @@
         <v>15.0</v>
       </c>
       <c r="V9" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="X9" t="n">
         <v>17.0</v>
       </c>
     </row>
@@ -23297,7 +23900,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="C10" t="n">
         <v>19.0</v>
@@ -23358,6 +23961,12 @@
       </c>
       <c r="V10" t="n">
         <v>11.0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="11">
@@ -23365,7 +23974,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C11" t="n">
         <v>13.0</v>
@@ -23425,6 +24034,12 @@
         <v>21.0</v>
       </c>
       <c r="V11" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="X11" t="n">
         <v>22.0</v>
       </c>
     </row>
@@ -23433,7 +24048,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C12" t="n">
         <v>20.0</v>
@@ -23493,7 +24108,13 @@
         <v>16.0</v>
       </c>
       <c r="V12" t="n">
-        <v>14.0</v>
+        <v>16.0</v>
+      </c>
+      <c r="W12" t="n">
+        <v>13.0</v>
+      </c>
+      <c r="X12" t="n">
+        <v>13.0</v>
       </c>
     </row>
     <row r="13">
@@ -23501,7 +24122,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C13" t="n">
         <v>21.0</v>
@@ -23562,6 +24183,12 @@
       </c>
       <c r="V13" t="n">
         <v>12.0</v>
+      </c>
+      <c r="W13" t="n">
+        <v>14.0</v>
+      </c>
+      <c r="X13" t="n">
+        <v>14.0</v>
       </c>
     </row>
     <row r="14">
@@ -23569,7 +24196,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C14" t="n">
         <v>14.0</v>
@@ -23629,6 +24256,12 @@
         <v>20.0</v>
       </c>
       <c r="V14" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="W14" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="X14" t="n">
         <v>20.0</v>
       </c>
     </row>
@@ -23637,7 +24270,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C15" t="n">
         <v>3.0</v>
@@ -23698,6 +24331,12 @@
       </c>
       <c r="V15" t="n">
         <v>2.0</v>
+      </c>
+      <c r="W15" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="X15" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="16">
@@ -23705,7 +24344,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="C16" t="n">
         <v>15.0</v>
@@ -23765,7 +24404,13 @@
         <v>22.0</v>
       </c>
       <c r="V16" t="n">
-        <v>21.0</v>
+        <v>22.0</v>
+      </c>
+      <c r="W16" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="X16" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="17">
@@ -23773,7 +24418,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C17" t="n">
         <v>4.0</v>
@@ -23834,6 +24479,12 @@
       </c>
       <c r="V17" t="n">
         <v>23.0</v>
+      </c>
+      <c r="W17" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="X17" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="18">
@@ -23841,7 +24492,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C18" t="n">
         <v>5.0</v>
@@ -23901,6 +24552,12 @@
         <v>7.0</v>
       </c>
       <c r="V18" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="W18" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="X18" t="n">
         <v>7.0</v>
       </c>
     </row>
@@ -23909,7 +24566,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C19" t="n">
         <v>22.0</v>
@@ -23969,6 +24626,12 @@
         <v>6.0</v>
       </c>
       <c r="V19" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="W19" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="X19" t="n">
         <v>6.0</v>
       </c>
     </row>
@@ -23977,7 +24640,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C20" t="n">
         <v>16.0</v>
@@ -24038,6 +24701,12 @@
       </c>
       <c r="V20" t="n">
         <v>24.0</v>
+      </c>
+      <c r="W20" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="X20" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="21">
@@ -24045,7 +24714,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C21" t="n">
         <v>6.0</v>
@@ -24106,6 +24775,12 @@
       </c>
       <c r="V21" t="n">
         <v>13.0</v>
+      </c>
+      <c r="W21" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="X21" t="n">
+        <v>11.0</v>
       </c>
     </row>
     <row r="22">
@@ -24113,7 +24788,7 @@
         <v>120</v>
       </c>
       <c r="B22" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C22" t="n">
         <v>23.0</v>
@@ -24173,6 +24848,12 @@
         <v>4.0</v>
       </c>
       <c r="V22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="W22" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="X22" t="n">
         <v>4.0</v>
       </c>
     </row>
@@ -24181,7 +24862,7 @@
         <v>121</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C23" t="n">
         <v>7.0</v>
@@ -24242,6 +24923,12 @@
       </c>
       <c r="V23" t="n">
         <v>1.0</v>
+      </c>
+      <c r="W23" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="X23" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="24">
@@ -24249,7 +24936,7 @@
         <v>122</v>
       </c>
       <c r="B24" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="C24" t="n">
         <v>24.0</v>
@@ -24309,6 +24996,12 @@
         <v>19.0</v>
       </c>
       <c r="V24" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="W24" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="X24" t="n">
         <v>19.0</v>
       </c>
     </row>
@@ -24317,7 +25010,7 @@
         <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C25" t="n">
         <v>8.0</v>
@@ -24377,7 +25070,13 @@
         <v>13.0</v>
       </c>
       <c r="V25" t="n">
-        <v>15.0</v>
+        <v>17.0</v>
+      </c>
+      <c r="W25" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="X25" t="n">
+        <v>18.0</v>
       </c>
     </row>
   </sheetData>
@@ -24396,7 +25095,7 @@
     <row r="1">
       <c r="A1"/>
       <c r="B1" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -24449,7 +25148,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C2" t="n">
         <v>13.0</v>
@@ -24502,7 +25201,7 @@
         <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C3" t="n">
         <v>9.0</v>
@@ -24555,7 +25254,7 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C4" t="n">
         <v>14.0</v>
@@ -24608,7 +25307,7 @@
         <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C5" t="n">
         <v>15.0</v>
@@ -24661,7 +25360,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C6" t="n">
         <v>16.0</v>
@@ -24714,7 +25413,7 @@
         <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C7" t="n">
         <v>1.0</v>
@@ -24767,7 +25466,7 @@
         <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C8" t="n">
         <v>2.0</v>
@@ -24820,7 +25519,7 @@
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C9" t="n">
         <v>3.0</v>
@@ -24873,7 +25572,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C10" t="n">
         <v>4.0</v>
@@ -24926,7 +25625,7 @@
         <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C11" t="n">
         <v>5.0</v>
@@ -24979,7 +25678,7 @@
         <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C12" t="n">
         <v>6.0</v>
@@ -25032,7 +25731,7 @@
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C13" t="n">
         <v>7.0</v>
@@ -25085,7 +25784,7 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C14" t="n">
         <v>10.0</v>
@@ -25138,7 +25837,7 @@
         <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C15" t="n">
         <v>11.0</v>
@@ -25191,7 +25890,7 @@
         <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C16" t="n">
         <v>8.0</v>
@@ -25244,7 +25943,7 @@
         <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C17" t="n">
         <v>17.0</v>
@@ -25297,7 +25996,7 @@
         <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C18" t="n">
         <v>18.0</v>
@@ -25350,7 +26049,7 @@
         <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C19" t="n">
         <v>19.0</v>
@@ -25403,7 +26102,7 @@
         <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C20" t="n">
         <v>12.0</v>
@@ -25456,7 +26155,7 @@
         <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C21" t="n">
         <v>20.0</v>

</xml_diff>